<commit_message>
getting ready to add second function
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/sensedComp1.xlsx
+++ b/shipClassTests/testResults/sensedComp1.xlsx
@@ -362,13 +362,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="4" width="12.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1">
-        <f>MODE(C[100, 0, 0, 3] : C[100, 0, 0, 3])</f>
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -414,13 +410,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -428,13 +424,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -442,13 +438,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -456,13 +452,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -470,13 +466,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -484,13 +480,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -498,13 +494,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -512,13 +508,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -526,13 +522,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -540,13 +536,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -554,13 +550,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -568,13 +564,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -582,13 +578,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -596,13 +592,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -610,13 +606,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -624,13 +620,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -638,13 +634,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -658,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -672,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -686,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -700,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -714,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -728,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -742,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -756,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -770,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -784,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -798,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -812,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -826,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -840,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -854,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -868,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -882,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -896,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -910,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -924,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -938,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -952,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -966,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -980,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -994,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1008,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1022,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1036,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1050,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1064,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1078,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1092,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1114,7 +1110,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1128,13 +1124,13 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1142,13 +1138,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1156,13 +1152,13 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1170,13 +1166,13 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1184,13 +1180,13 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1198,13 +1194,13 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1212,13 +1208,13 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1226,13 +1222,13 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1240,13 +1236,13 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1254,13 +1250,13 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1268,13 +1264,13 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1282,13 +1278,13 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1296,13 +1292,13 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1310,13 +1306,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1324,13 +1320,13 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1338,13 +1334,13 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1358,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1372,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1386,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1400,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1414,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1428,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1442,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1456,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1470,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1484,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1498,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1512,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1526,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1540,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1554,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1568,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1582,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1596,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1610,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1624,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1638,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1652,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1666,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1680,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1694,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1708,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1722,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1736,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1750,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1764,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1778,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1792,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding ship class and ship class output
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/sensedComp1.xlsx
+++ b/shipClassTests/testResults/sensedComp1.xlsx
@@ -76,8 +76,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,31 +382,31 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -434,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <f>IF(AND(H2=1, A2=F2), 1, 0)</f>
+        <f>IF(B2=G2, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -465,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f>IF(AND(H3=1, A3=F3), 1, 0)</f>
+        <f>IF(B3=G3, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -496,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f>IF(AND(H4=1, A4=F4), 1, 0)</f>
+        <f>IF(B4=G4, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -514,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -527,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <f>IF(AND(H5=1, A5=F5), 1, 0)</f>
+        <f>IF(B5=G5, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -545,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -558,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f>IF(AND(H6=1, A6=F6), 1, 0)</f>
+        <f>IF(B6=G6, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -576,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -589,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <f>IF(AND(H7=1, A7=F7), 1, 0)</f>
+        <f>IF(B7=G7, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -607,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -620,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f>IF(AND(H8=1, A8=F8), 1, 0)</f>
+        <f>IF(B8=G8, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -638,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -651,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f>IF(AND(H9=1, A9=F9), 1, 0)</f>
+        <f>IF(B9=G9, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -669,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -682,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f>IF(AND(H10=1, A10=F10), 1, 0)</f>
+        <f>IF(B10=G10, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -694,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -713,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>IF(AND(H11=1, A11=F11), 1, 0)</f>
+        <f>IF(B11=G11, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -725,16 +728,16 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -744,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(AND(H12=1, A12=F12), 1, 0)</f>
+        <f>IF(B12=G12, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -756,16 +759,16 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -775,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IF(AND(H13=1, A13=F13), 1, 0)</f>
+        <f>IF(B13=G13, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -787,16 +790,16 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -806,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IF(AND(H14=1, A14=F14), 1, 0)</f>
+        <f>IF(B14=G14, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -818,16 +821,16 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -837,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f>IF(AND(H15=1, A15=F15), 1, 0)</f>
+        <f>IF(B15=G15, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -855,10 +858,10 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -868,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IF(AND(H16=1, A16=F16), 1, 0)</f>
+        <f>IF(B16=G16, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -886,10 +889,10 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -899,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <f>IF(AND(H17=1, A17=F17), 1, 0)</f>
+        <f>IF(B17=G17, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -917,10 +920,10 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -930,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <f>IF(AND(H18=1, A18=F18), 1, 0)</f>
+        <f>IF(B18=G18, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -948,10 +951,10 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -961,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <f>IF(AND(H19=1, A19=F19), 1, 0)</f>
+        <f>IF(B19=G19, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -979,10 +982,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -992,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <f>IF(AND(H20=1, A20=F20), 1, 0)</f>
+        <f>IF(B20=G20, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1010,10 +1013,10 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1023,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f>IF(AND(H21=1, A21=F21), 1, 0)</f>
+        <f>IF(B21=G21, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1041,10 +1044,10 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1054,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <f>IF(AND(H22=1, A22=F22), 1, 0)</f>
+        <f>IF(B22=G22, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1072,10 +1075,10 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1085,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f>IF(AND(H23=1, A23=F23), 1, 0)</f>
+        <f>IF(B23=G23, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1103,10 +1106,10 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1116,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f>IF(AND(H24=1, A24=F24), 1, 0)</f>
+        <f>IF(B24=G24, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1134,10 +1137,10 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1147,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <f>IF(AND(H25=1, A25=F25), 1, 0)</f>
+        <f>IF(B25=G25, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1165,10 +1168,10 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1178,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f>IF(AND(H26=1, A26=F26), 1, 0)</f>
+        <f>IF(B26=G26, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1196,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1209,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>IF(AND(H27=1, A27=F27), 1, 0)</f>
+        <f>IF(B27=G27, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1227,10 +1230,10 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1240,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f>IF(AND(H28=1, A28=F28), 1, 0)</f>
+        <f>IF(B28=G28, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1258,10 +1261,10 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1271,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f>IF(AND(H29=1, A29=F29), 1, 0)</f>
+        <f>IF(B29=G29, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1289,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1302,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f>IF(AND(H30=1, A30=F30), 1, 0)</f>
+        <f>IF(B30=G30, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1320,10 +1323,10 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1333,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <f>IF(AND(H31=1, A31=F31), 1, 0)</f>
+        <f>IF(B31=G31, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1351,10 +1354,10 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1364,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <f>IF(AND(H32=1, A32=F32), 1, 0)</f>
+        <f>IF(B32=G32, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1382,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1395,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <f>IF(AND(H33=1, A33=F33), 1, 0)</f>
+        <f>IF(B33=G33, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1413,10 +1416,10 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1426,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <f>IF(AND(H34=1, A34=F34), 1, 0)</f>
+        <f>IF(B34=G34, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1444,10 +1447,10 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1457,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <f>IF(AND(H35=1, A35=F35), 1, 0)</f>
+        <f>IF(B35=G35, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1475,10 +1478,10 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1488,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <f>IF(AND(H36=1, A36=F36), 1, 0)</f>
+        <f>IF(B36=G36, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1506,10 +1509,10 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1519,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <f>IF(AND(H37=1, A37=F37), 1, 0)</f>
+        <f>IF(B37=G37, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1537,10 +1540,10 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1550,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <f>IF(AND(H38=1, A38=F38), 1, 0)</f>
+        <f>IF(B38=G38, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1568,10 +1571,10 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -1581,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <f>IF(AND(H39=1, A39=F39), 1, 0)</f>
+        <f>IF(B39=G39, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1599,10 +1602,10 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1612,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <f>IF(AND(H40=1, A40=F40), 1, 0)</f>
+        <f>IF(B40=G40, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1630,10 +1633,10 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1643,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <f>IF(AND(H41=1, A41=F41), 1, 0)</f>
+        <f>IF(B41=G41, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1661,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1674,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <f>IF(AND(H42=1, A42=F42), 1, 0)</f>
+        <f>IF(B42=G42, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1692,10 +1695,10 @@
         <v>1</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1705,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <f>IF(AND(H43=1, A43=F43), 1, 0)</f>
+        <f>IF(B43=G43, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1723,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -1736,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <f>IF(AND(H44=1, A44=F44), 1, 0)</f>
+        <f>IF(B44=G44, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1754,10 +1757,10 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1767,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <f>IF(AND(H45=1, A45=F45), 1, 0)</f>
+        <f>IF(B45=G45, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1785,10 +1788,10 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -1798,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <f>IF(AND(H46=1, A46=F46), 1, 0)</f>
+        <f>IF(B46=G46, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1816,10 +1819,10 @@
         <v>1</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1829,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <f>IF(AND(H47=1, A47=F47), 1, 0)</f>
+        <f>IF(B47=G47, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1847,10 +1850,10 @@
         <v>1</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1860,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <f>IF(AND(H48=1, A48=F48), 1, 0)</f>
+        <f>IF(B48=G48, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1878,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1891,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <f>IF(AND(H49=1, A49=F49), 1, 0)</f>
+        <f>IF(B49=G49, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1909,10 +1912,10 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -1922,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <f>IF(AND(H50=1, A50=F50), 1, 0)</f>
+        <f>IF(B50=G50, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1940,10 +1943,10 @@
         <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -1953,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <f>IF(AND(H51=1, A51=F51), 1, 0)</f>
+        <f>IF(B51=G51, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1971,10 +1974,10 @@
         <v>1</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -1984,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <f>IF(AND(H52=1, A52=F52), 1, 0)</f>
+        <f>IF(B52=G52, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2002,10 +2005,10 @@
         <v>1</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2015,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <f>IF(AND(H53=1, A53=F53), 1, 0)</f>
+        <f>IF(B53=G53, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2033,10 +2036,10 @@
         <v>1</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2046,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <f>IF(AND(H54=1, A54=F54), 1, 0)</f>
+        <f>IF(B54=G54, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2064,10 +2067,10 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2077,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <f>IF(AND(H55=1, A55=F55), 1, 0)</f>
+        <f>IF(B55=G55, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2095,10 +2098,10 @@
         <v>1</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2108,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <f>IF(AND(H56=1, A56=F56), 1, 0)</f>
+        <f>IF(B56=G56, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2126,10 +2129,10 @@
         <v>1</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2139,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <f>IF(AND(H57=1, A57=F57), 1, 0)</f>
+        <f>IF(B57=G57, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2157,10 +2160,10 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2170,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <f>IF(AND(H58=1, A58=F58), 1, 0)</f>
+        <f>IF(B58=G58, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2188,10 +2191,10 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2201,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <f>IF(AND(H59=1, A59=F59), 1, 0)</f>
+        <f>IF(B59=G59, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2219,10 +2222,10 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2232,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <f>IF(AND(H60=1, A60=F60), 1, 0)</f>
+        <f>IF(B60=G60, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2250,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2263,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <f>IF(AND(H61=1, A61=F61), 1, 0)</f>
+        <f>IF(B61=G61, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2281,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2294,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <f>IF(AND(H62=1, A62=F62), 1, 0)</f>
+        <f>IF(B62=G62, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2325,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f>IF(AND(H63=1, A63=F63), 1, 0)</f>
+        <f>IF(B63=G63, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2356,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <f>IF(AND(H64=1, A64=F64), 1, 0)</f>
+        <f>IF(B64=G64, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2374,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2387,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <f>IF(AND(H65=1, A65=F65), 1, 0)</f>
+        <f>IF(B65=G65, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2405,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2418,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <f>IF(AND(H66=1, A66=F66), 1, 0)</f>
+        <f>IF(B66=G66, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2436,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2449,7 +2452,7 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <f>IF(AND(H67=1, A67=F67), 1, 0)</f>
+        <f>IF(B67=G67, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2467,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2480,7 +2483,7 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <f>IF(AND(H68=1, A68=F68), 1, 0)</f>
+        <f>IF(B68=G68, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2498,7 +2501,7 @@
         <v>1</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2511,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <f>IF(AND(H69=1, A69=F69), 1, 0)</f>
+        <f>IF(B69=G69, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2529,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2542,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="I70">
-        <f>IF(AND(H70=1, A70=F70), 1, 0)</f>
+        <f>IF(B70=G70, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2554,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2573,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <f>IF(AND(H71=1, A71=F71), 1, 0)</f>
+        <f>IF(B71=G71, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2585,16 +2588,16 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -2604,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <f>IF(AND(H72=1, A72=F72), 1, 0)</f>
+        <f>IF(B72=G72, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2616,16 +2619,16 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -2635,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="I73">
-        <f>IF(AND(H73=1, A73=F73), 1, 0)</f>
+        <f>IF(B73=G73, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2647,16 +2650,16 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2666,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <f>IF(AND(H74=1, A74=F74), 1, 0)</f>
+        <f>IF(B74=G74, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2678,16 +2681,16 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -2697,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="I75">
-        <f>IF(AND(H75=1, A75=F75), 1, 0)</f>
+        <f>IF(B75=G75, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2715,10 +2718,10 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -2728,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="I76">
-        <f>IF(AND(H76=1, A76=F76), 1, 0)</f>
+        <f>IF(B76=G76, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2746,10 +2749,10 @@
         <v>1</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -2759,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="I77">
-        <f>IF(AND(H77=1, A77=F77), 1, 0)</f>
+        <f>IF(B77=G77, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2777,10 +2780,10 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -2790,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="I78">
-        <f>IF(AND(H78=1, A78=F78), 1, 0)</f>
+        <f>IF(B78=G78, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2808,10 +2811,10 @@
         <v>1</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -2821,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="I79">
-        <f>IF(AND(H79=1, A79=F79), 1, 0)</f>
+        <f>IF(B79=G79, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2839,10 +2842,10 @@
         <v>1</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -2852,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <f>IF(AND(H80=1, A80=F80), 1, 0)</f>
+        <f>IF(B80=G80, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2870,10 +2873,10 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2883,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="I81">
-        <f>IF(AND(H81=1, A81=F81), 1, 0)</f>
+        <f>IF(B81=G81, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2901,10 +2904,10 @@
         <v>1</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2914,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <f>IF(AND(H82=1, A82=F82), 1, 0)</f>
+        <f>IF(B82=G82, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2932,10 +2935,10 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2945,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="I83">
-        <f>IF(AND(H83=1, A83=F83), 1, 0)</f>
+        <f>IF(B83=G83, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2963,10 +2966,10 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -2976,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <f>IF(AND(H84=1, A84=F84), 1, 0)</f>
+        <f>IF(B84=G84, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2994,10 +2997,10 @@
         <v>1</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3007,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="I85">
-        <f>IF(AND(H85=1, A85=F85), 1, 0)</f>
+        <f>IF(B85=G85, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3025,10 +3028,10 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -3038,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="I86">
-        <f>IF(AND(H86=1, A86=F86), 1, 0)</f>
+        <f>IF(B86=G86, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3056,10 +3059,10 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -3069,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="I87">
-        <f>IF(AND(H87=1, A87=F87), 1, 0)</f>
+        <f>IF(B87=G87, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3087,10 +3090,10 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -3100,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="I88">
-        <f>IF(AND(H88=1, A88=F88), 1, 0)</f>
+        <f>IF(B88=G88, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3118,10 +3121,10 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3131,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <f>IF(AND(H89=1, A89=F89), 1, 0)</f>
+        <f>IF(B89=G89, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3149,10 +3152,10 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3162,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="I90">
-        <f>IF(AND(H90=1, A90=F90), 1, 0)</f>
+        <f>IF(B90=G90, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3180,10 +3183,10 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3193,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="I91">
-        <f>IF(AND(H91=1, A91=F91), 1, 0)</f>
+        <f>IF(B91=G91, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3211,10 +3214,10 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3224,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <f>IF(AND(H92=1, A92=F92), 1, 0)</f>
+        <f>IF(B92=G92, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3242,10 +3245,10 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="I93">
-        <f>IF(AND(H93=1, A93=F93), 1, 0)</f>
+        <f>IF(B93=G93, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3273,10 +3276,10 @@
         <v>1</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3286,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="I94">
-        <f>IF(AND(H94=1, A94=F94), 1, 0)</f>
+        <f>IF(B94=G94, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3304,10 +3307,10 @@
         <v>1</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3317,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="I95">
-        <f>IF(AND(H95=1, A95=F95), 1, 0)</f>
+        <f>IF(B95=G95, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3335,10 +3338,10 @@
         <v>1</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -3348,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <f>IF(AND(H96=1, A96=F96), 1, 0)</f>
+        <f>IF(B96=G96, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3366,10 +3369,10 @@
         <v>1</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3379,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="I97">
-        <f>IF(AND(H97=1, A97=F97), 1, 0)</f>
+        <f>IF(B97=G97, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3397,10 +3400,10 @@
         <v>1</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3410,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="I98">
-        <f>IF(AND(H98=1, A98=F98), 1, 0)</f>
+        <f>IF(B98=G98, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3428,10 +3431,10 @@
         <v>1</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -3441,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="I99">
-        <f>IF(AND(H99=1, A99=F99), 1, 0)</f>
+        <f>IF(B99=G99, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3459,10 +3462,10 @@
         <v>1</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3472,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="I100">
-        <f>IF(AND(H100=1, A100=F100), 1, 0)</f>
+        <f>IF(B100=G100, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3490,10 +3493,10 @@
         <v>1</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3503,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="I101">
-        <f>IF(AND(H101=1, A101=F101), 1, 0)</f>
+        <f>IF(B101=G101, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3521,10 +3524,10 @@
         <v>1</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -3534,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <f>IF(AND(H102=1, A102=F102), 1, 0)</f>
+        <f>IF(B102=G102, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3552,10 +3555,10 @@
         <v>1</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -3565,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <f>IF(AND(H103=1, A103=F103), 1, 0)</f>
+        <f>IF(B103=G103, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3583,10 +3586,10 @@
         <v>1</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -3596,7 +3599,7 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <f>IF(AND(H104=1, A104=F104), 1, 0)</f>
+        <f>IF(B104=G104, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3614,10 +3617,10 @@
         <v>1</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -3627,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <f>IF(AND(H105=1, A105=F105), 1, 0)</f>
+        <f>IF(B105=G105, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3645,10 +3648,10 @@
         <v>1</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3658,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <f>IF(AND(H106=1, A106=F106), 1, 0)</f>
+        <f>IF(B106=G106, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3676,10 +3679,10 @@
         <v>1</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -3689,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="I107">
-        <f>IF(AND(H107=1, A107=F107), 1, 0)</f>
+        <f>IF(B107=G107, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3707,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -3720,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="I108">
-        <f>IF(AND(H108=1, A108=F108), 1, 0)</f>
+        <f>IF(B108=G108, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3738,10 +3741,10 @@
         <v>1</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -3751,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="I109">
-        <f>IF(AND(H109=1, A109=F109), 1, 0)</f>
+        <f>IF(B109=G109, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3769,10 +3772,10 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3782,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="I110">
-        <f>IF(AND(H110=1, A110=F110), 1, 0)</f>
+        <f>IF(B110=G110, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3800,10 +3803,10 @@
         <v>1</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -3813,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="I111">
-        <f>IF(AND(H111=1, A111=F111), 1, 0)</f>
+        <f>IF(B111=G111, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3831,10 +3834,10 @@
         <v>1</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -3844,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="I112">
-        <f>IF(AND(H112=1, A112=F112), 1, 0)</f>
+        <f>IF(B112=G112, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3862,10 +3865,10 @@
         <v>1</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3875,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="I113">
-        <f>IF(AND(H113=1, A113=F113), 1, 0)</f>
+        <f>IF(B113=G113, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3893,10 +3896,10 @@
         <v>1</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -3906,7 +3909,7 @@
         <v>0</v>
       </c>
       <c r="I114">
-        <f>IF(AND(H114=1, A114=F114), 1, 0)</f>
+        <f>IF(B114=G114, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3924,10 +3927,10 @@
         <v>1</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -3937,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="I115">
-        <f>IF(AND(H115=1, A115=F115), 1, 0)</f>
+        <f>IF(B115=G115, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3955,10 +3958,10 @@
         <v>1</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -3968,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="I116">
-        <f>IF(AND(H116=1, A116=F116), 1, 0)</f>
+        <f>IF(B116=G116, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3986,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3999,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="I117">
-        <f>IF(AND(H117=1, A117=F117), 1, 0)</f>
+        <f>IF(B117=G117, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4017,10 +4020,10 @@
         <v>1</v>
       </c>
       <c r="E118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4030,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="I118">
-        <f>IF(AND(H118=1, A118=F118), 1, 0)</f>
+        <f>IF(B118=G118, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4048,10 +4051,10 @@
         <v>1</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4061,7 +4064,7 @@
         <v>0</v>
       </c>
       <c r="I119">
-        <f>IF(AND(H119=1, A119=F119), 1, 0)</f>
+        <f>IF(B119=G119, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4079,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4092,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="I120">
-        <f>IF(AND(H120=1, A120=F120), 1, 0)</f>
+        <f>IF(B120=G120, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4110,10 +4113,10 @@
         <v>1</v>
       </c>
       <c r="E121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -4123,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="I121">
-        <f>IF(AND(H121=1, A121=F121), 1, 0)</f>
+        <f>IF(B121=G121, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4141,10 +4144,10 @@
         <v>1</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4154,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="I122">
-        <f>IF(AND(H122=1, A122=F122), 1, 0)</f>
+        <f>IF(B122=G122, 1, 0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>